<commit_message>
notes for day1 and day2
</commit_message>
<xml_diff>
--- a/PPP_literauture/literature_updates.xlsx
+++ b/PPP_literauture/literature_updates.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>Automotive &amp; EV digital twins</t>
+  </si>
+  <si>
+    <t>https://www.spglobal.com/automotive-insights/en/blogs/2025/08/digital-twins-in-the-automotive-industry-explained?utm_source=chatgpt.com</t>
   </si>
   <si>
     <t>28-Sept</t>
@@ -363,7 +366,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,12 +381,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.15"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -599,7 +596,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -623,7 +620,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="thin">
@@ -641,7 +651,7 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="medium">
@@ -653,34 +663,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -690,9 +676,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left/>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -703,10 +687,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
@@ -716,28 +700,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -968,7 +952,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -980,144 +964,144 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1126,46 +1110,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1701,13 +1682,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:E27"/>
+  <dimension ref="B1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="7.88888888888889" customWidth="1"/>
     <col min="3" max="3" width="85.4444444444444" customWidth="1"/>
@@ -1716,6 +1697,7 @@
     <col min="6" max="6" width="22.7777777777778" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="15.15"/>
     <row r="2" ht="15.15" spans="2:5">
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1757,237 +1739,240 @@
       </c>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="2:6">
+      <c r="B12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>14</v>
       </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="C13" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="D13" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="B14" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="C14" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="D14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="16" t="s">
+      <c r="B15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="D15" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>45931</v>
       </c>
-      <c r="C16" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="14" t="s">
+      <c r="C16" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="D16" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:5">
-      <c r="B17" s="17">
+      <c r="B17" s="16">
         <v>45932</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="14" t="s">
+      <c r="C17" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="D17" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:5">
-      <c r="B18" s="17">
+      <c r="B18" s="16">
         <v>45933</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="14" t="s">
+      <c r="C18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" ht="15.15" spans="2:5">
-      <c r="B19" s="17">
+      <c r="B19" s="16">
         <v>45934</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="19" t="s">
+      <c r="C19" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="D19" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" ht="15.15" spans="2:2">
-      <c r="B20" s="21">
+      <c r="B20" s="20">
         <v>45935</v>
       </c>
     </row>
     <row r="22" spans="3:3">
-      <c r="C22" s="14" t="s">
-        <v>53</v>
+      <c r="C22" s="13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="4:4">
-      <c r="D25" s="22" t="s">
+      <c r="D25" s="21" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="4:4">
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="27" spans="4:4">
-      <c r="D27" s="24" t="s">
+      <c r="D27" s="23" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>